<commit_message>
Listed all accessories products
</commit_message>
<xml_diff>
--- a/Assets/Products Team/Products data.xlsx
+++ b/Assets/Products Team/Products data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b6e5e365387d49b/Documents/GitHub/Mahalaxmi-Enterprises-Tailwind-Version/Assets/Products Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_F25DC773A252ABDACC1048B8915E607E5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B85AADF7-3BB9-4B46-81C9-C1FE0ACFA890}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC1048B8915E607E5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D433DE8-A3B9-4FF9-80D1-4305734E75C1}"/>
   <bookViews>
-    <workbookView xWindow="-615" yWindow="1140" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mobile &amp; Computer Accessories" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t>Product ID</t>
   </si>
@@ -319,13 +319,147 @@
     <t>Rechargable metal keychain with light</t>
   </si>
   <si>
-    <t>Listing status</t>
-  </si>
-  <si>
     <t>Listed</t>
   </si>
   <si>
     <t>Color Pods</t>
+  </si>
+  <si>
+    <t>Feature head points</t>
+  </si>
+  <si>
+    <t>Here’s the description in point format:
+- **Enhanced Noise Cancellation**: Provides up to **2x more Active Noise Cancellation** than the previous model.
+- **Adaptive Audio**: Dynamically adjusts noise control based on your environment.
+- **Personalized Spatial Audio**: Creates a more immersive sound experience tailored to the user.
+- **Custom-Built Driver &amp; Amplifier**: Delivers **rich, high-quality sound**.
+- **Touch Control**: Allows **easy volume adjustments** with simple touch gestures.
+This format makes the key features stand out more clearly! Let me know if you’d like further refinements.</t>
+  </si>
+  <si>
+    <t>Here are the key features of **Color Pods** in a structured format:
+### **Key Features of Color Pods**  
+- **Sleek &amp; Ergonomic Design** – Stylish and comfortable fit for all-day wear.  
+- **Immersive Sound Quality** – Delivers rich, high-fidelity audio for an enhanced listening experience.  
+- **Active Noise Cancellation** – Blocks out distractions for crystal-clear sound and calls.  
+- **Vibrant Color Options** – Available in multiple shades to match your style and personality.  
+- **Touch Controls** – Effortlessly adjust volume, playback, and calls with simple touch gestures.  
+- **Long-Lasting Battery Life** – Extended usage with a reliable power reserve.  
+- **Compact Charging Case** – Easily portable for convenient recharging on the go.  
+This structure makes the features pop while keeping them clear and concise. Let me know if you'd like any refinements!</t>
+  </si>
+  <si>
+    <t>### **Key Features of the 3.5mm to USB-C Dongle**  
+- **Seamless Connectivity** – Connects wired headphones to modern devices without a headphone jack.  
+- **High-Fidelity Audio** – Ensures crystal-clear sound transmission for an immersive listening experience.  
+- **Universal Compatibility** – Works with smartphones, tablets, and laptops featuring a USB-C port.  
+- **Durable Build** – Designed for longevity and reliable performance.  
+- **Plug-and-Play Functionality** – No additional setup required—just connect and enjoy.  
+- **Lightweight &amp; Compact** – Portable design makes it easy to carry and use anywhere.  
+This keeps the features clear and structured for quick reference. Let me know if you'd like any tweaks!</t>
+  </si>
+  <si>
+    <t>### **Key Features of the USB Type-C Fast Charging Cable**  
+- **High-Speed Power Delivery** – Supports fast charging protocols for quick and efficient power supply.  
+- **Reliable Data Transfer** – Enables seamless file transfers with enhanced speed and stability.  
+- **Durable Construction** – Made with sturdy materials for long-lasting performance.  
+- **Reversible Connector** – Hassle-free plugging in either orientation.  
+- **Universal Compatibility** – Works with smartphones, tablets, laptops, and other USB-C devices.  
+- **Compact &amp; Convenient** – Lightweight design for easy portability and everyday use.  
+This format keeps the key points concise and impactful. Let me know if you need any refinements!</t>
+  </si>
+  <si>
+    <t>### **Key Features of the Bluetooth Mini Speaker**  
+- **Compact &amp; Powerful Sound** – Delivers impressive audio quality in a small, portable design.  
+- **Wireless Connectivity** – Seamless Bluetooth pairing for hassle-free listening.  
+- **Durable &amp; Portable Build** – Designed for easy travel and long-lasting use.  
+- **Clear Bass &amp; Crisp Audio** – Ensures rich sound performance across all frequencies.  
+- **Long-Lasting Battery** – Extended playback time for uninterrupted enjoyment.  
+- **Intuitive Controls** – Effortless volume, playback, and pairing management.  
+This format keeps the key selling points clear and engaging! Let me know if you need any refinements.</t>
+  </si>
+  <si>
+    <t>### **Key Features of the 20W USB-C Charger**  
+- **Fast &amp; Efficient Charging** – Provides rapid power delivery for minimal downtime.  
+- **Universal USB-C Compatibility** – Works seamlessly with smartphones, tablets, and accessories.  
+- **Compact &amp; Portable Design** – Easy to carry, perfect for travel and everyday use.  
+- **Smart Power Management** – Prevents overheating and ensures reliable performance.  
+- **Seamless Power Delivery** – Just pair with your preferred USB-C cable for instant charging.  
+This format keeps the key details clear and engaging. Let me know if you’d like any refinements!</t>
+  </si>
+  <si>
+    <t>### **Key Features of Wired Earphones with Lightning Port**  
+- **High-Quality Audio** – Delivers clear and immersive sound for music, calls, and podcasts.  
+- **Seamless Connectivity** – Lightning connector ensures stable, lag-free transmission.  
+- **Noise Isolation** – Minimizes external distractions for an enhanced listening experience.  
+- **Ergonomic Fit** – Designed for comfort, making them perfect for extended wear.  
+- **Inline Remote** – Easily manage volume, playback, and calls with built-in controls.  
+- **Durable Build** – Reliable and sturdy construction for long-term use.  
+- **Plug-and-Play Convenience** – No additional setup required—just connect and enjoy.  
+This format keeps the features structured and impactful. Let me know if you'd like any adjustments!</t>
+  </si>
+  <si>
+    <t>### **Key Features of the Micro USB/V8 Cable**  
+- **Reliable Charging &amp; Data Transfer** – Ensures efficient power delivery and seamless syncing.  
+- **Stable Connectivity** – Designed for micro USB-compatible devices, including older-generation smartphones and tablets.  
+- **Durable Build** – Sturdy materials provide long-lasting performance.  
+- **Fast Charging Support** – Delivers quick and reliable power supply.  
+- **Compact &amp; Travel-Friendly** – Lightweight design makes it easy to carry and use anywhere.  
+This keeps the features structured and easy to grasp! Let me know if you need any tweaks.</t>
+  </si>
+  <si>
+    <t>### **Key Features of the USB-A to Type-C Cable**  
+- **Versatile Charging &amp; Data Transfer** – Bridges legacy USB-A ports with modern USB-C devices.  
+- **Fast &amp; Reliable Power Delivery** – Ensures quick and efficient charging.  
+- **Universal Compatibility** – Works seamlessly with smartphones, tablets, laptops, and more.  
+- **Durable Build** – Designed for longevity and stable performance.  
+- **Reversible Type-C Connector** – Hassle-free plugging in either orientation.  
+- **Perfect for All Environments** – Ideal for home, office, or travel use.  
+This format keeps the features crisp and engaging! Let me know if you need any refinements.</t>
+  </si>
+  <si>
+    <t>### **Key Features of the 1W USB Bulb**  
+- **Compact &amp; Energy-Efficient** – Provides bright illumination with minimal power consumption.  
+- **USB-Powered Convenience** – Plugs into laptops, power banks, or adapters for instant use.  
+- **Bright &amp; Steady Light** – Reliable brightness despite its low power rating.  
+- **Versatile Usage** – Ideal for camping, travel, emergency lighting, or workspace enhancement.  
+- **Lightweight &amp; Durable Design** – Easy to carry and built for long-term reliability.  
+- **Plug-and-Play Functionality** – No setup required—just connect and illuminate.  
+This keeps the features structured and easy to digest. Let me know if you’d like any refinements!</t>
+  </si>
+  <si>
+    <t>### **Key Features of the Flexible USB Keyboard**  
+- **Durable &amp; Lightweight** – Designed for portability without compromising reliability.  
+- **Spill-Resistant &amp; Waterproof** – Protects against accidental spills and dust for long-lasting use.  
+- **Soft Silicone Material** – Offers a silent and comfortable typing experience.  
+- **Roll-Up Design** – Easily stores and carries for travel-friendly convenience.  
+- **Plug-and-Play USB Connectivity** – Works seamlessly with laptops, desktops, and tablets.  
+- **Versatile Usage** – Ideal for work, gaming, or everyday on-the-go tasks.  
+This layout keeps the features clear and engaging! Let me know if you’d like any adjustments.</t>
+  </si>
+  <si>
+    <t>### **Key Features of the 4-in-1 USB 3.0 Hub**  
+- **Expanded Connectivity** – Provides four high-speed USB 3.0 ports for multiple peripherals.  
+- **Fast Data Transfer** – Supports speeds up to **5Gbps** for quick access to external storage and accessories.  
+- **Compact &amp; Lightweight** – Easy to carry, perfect for home, office, and travel use.  
+- **Plug-and-Play Compatibility** – No drivers needed—just connect and start using.  
+- **Versatile Usage** – Ideal for connecting a mouse, keyboard, flash drive, external hard drive, and more.  
+This format keeps the details clear and engaging! Let me know if you'd like any refinements.</t>
+  </si>
+  <si>
+    <t>### **Key Features of the Foldable Metal Laptop Stand**  
+- **Durable Metal Construction** – Provides stability and reliable support for laptops.  
+- **Efficient Heat Dissipation** – Helps maintain optimal laptop performance.  
+- **Ergonomic Adjustable Angles** – Reduces strain on your neck and wrists for better posture.  
+- **Portable &amp; Foldable Design** – Easily fits into bags for convenience on the go.  
+- **Versatile Usage** – Ideal for work, study, gaming, or casual use in any setting.  
+This structure keeps the features concise and engaging! Let me know if you need any tweaks.</t>
+  </si>
+  <si>
+    <t>Listing status (under category page)</t>
+  </si>
+  <si>
+    <t>Listing status (actual product page)</t>
   </si>
 </sst>
 </file>
@@ -412,12 +546,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,22 +836,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -724,19 +863,25 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -746,43 +891,55 @@
       <c r="C2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4">
         <v>2999</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>999</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="4">
         <v>1499</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>799</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -792,20 +949,26 @@
       <c r="C4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="4">
         <v>999</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>499</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -815,20 +978,26 @@
       <c r="C5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="4">
         <v>999</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>449</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -838,20 +1007,26 @@
       <c r="C6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="4">
         <v>2499</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>1299</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -861,20 +1036,26 @@
       <c r="C7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="4">
         <v>1999</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>1499</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -884,20 +1065,26 @@
       <c r="C8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="4">
         <v>3999</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="4">
         <v>999</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -907,20 +1094,24 @@
       <c r="C9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="4">
         <v>499</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>249</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -930,20 +1121,24 @@
       <c r="C10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="4">
         <v>699</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>449</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -953,20 +1148,24 @@
       <c r="C11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="4">
         <v>199</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>149</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -976,20 +1175,24 @@
       <c r="C12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="4">
         <v>1999</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="4">
         <v>549</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -999,20 +1202,24 @@
       <c r="C13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="4">
         <v>999</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>799</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -1022,18 +1229,22 @@
       <c r="C14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="4">
         <v>1499</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>999</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="H14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1050,17 +1261,17 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1100,7 +1311,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -1120,7 +1331,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>59</v>
       </c>
@@ -1140,7 +1351,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
@@ -1160,7 +1371,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>61</v>
       </c>
@@ -1180,7 +1391,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>62</v>
       </c>
@@ -1200,7 +1411,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>63</v>
       </c>
@@ -1220,7 +1431,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>64</v>
       </c>
@@ -1240,7 +1451,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>65</v>
       </c>
@@ -1260,7 +1471,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Listed all gadgets products
</commit_message>
<xml_diff>
--- a/Assets/Products Team/Products data.xlsx
+++ b/Assets/Products Team/Products data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b6e5e365387d49b/Documents/GitHub/Mahalaxmi-Enterprises-Tailwind-Version/Assets/Products Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC1048B8915E607E5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D433DE8-A3B9-4FF9-80D1-4305734E75C1}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC1048B8915E607E5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96ADC8CA-BE27-4E7B-80C3-1231AE0A6006}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mobile &amp; Computer Accessories" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="126">
   <si>
     <t>Product ID</t>
   </si>
@@ -460,6 +460,100 @@
   </si>
   <si>
     <t>Listing status (actual product page)</t>
+  </si>
+  <si>
+    <t>Features head point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are key feature head points for your rechargeable torch:  
+- **USB Rechargeable** – Convenient and fast charging with included cable  
+- **Ergonomic Grip** – Designed for comfort and easy handling  
+- **Bright Illumination** – Powerful beam for clear visibility in the dark  
+- **Versatile Use** – Ideal for outdoor activities, emergencies, and daily needs  
+- **Durable Build** – Long-lasting and reliable performance  
+Let me know if you'd like further refinements!  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are concise and impactful head points for your calculation assistance request:  
+- **Math Support** – Get help with basic and complex equations  
+- **Arithmetic &amp; Percentages** – Solve everyday numerical problems effortlessly  
+- **Problem-Solving** – Assistance with step-by-step calculations  
+- **Quick &amp; Accurate** – Reliable solutions tailored to your needs  
+- **Versatile Help** – From simple math to advanced computations  
+Let me know if you'd like any refinements!  </t>
+  </si>
+  <si>
+    <t>Here are sharp and compelling feature head points for your rechargeable torch with a holder:  
+- **Powerful Illumination** – Bright beam for exploring, camping &amp; emergencies  
+- **Hands-Free Convenience** – Secure holder for easy placement &amp; usability  
+- **USB Rechargeable** – Hassle-free charging for reliable performance  
+- **Durable Build** – Designed for long-lasting use in any situation  
+- **Versatile Companion** – Ideal for outdoor adventures &amp; everyday needs  
+Let me know if you’d like any refinements!</t>
+  </si>
+  <si>
+    <t>Here are sharp and engaging feature head points for your advanced trimmer:  
+- **Precision Grooming** – Achieve effortless styling with accurate trimming  
+- **Built-in Digital Meter** – Real-time updates on battery life &amp; performance  
+- **Versatile Usage** – Ideal for facial hair, beards &amp; hairstyling needs  
+- **Compact &amp; Sleek Design** – User-friendly and travel-ready convenience  
+- **Tailored Experience** – Adjustable settings for personalized grooming  
+Let me know if you'd like any refinements!</t>
+  </si>
+  <si>
+    <t>Here are sharp and compelling feature head points for your rechargeable metal keychain:  
+- **Built-in LED Light** – Bright illumination for night-time convenience  
+- **Durable Metal Design** – Sleek, lightweight &amp; perfect for everyday carry  
+- **USB Rechargeable** – Eco-friendly &amp; battery-saving functionality  
+- **Compact &amp; Stylish** – A practical accessory with a modern look  
+- **Reliable Utility** – Ideal for unlocking doors &amp; navigating dark spaces  
+Let me know if you’d like any refinements!</t>
+  </si>
+  <si>
+    <t>Here are impactful feature head points for your handheld megaphone:  
+- **Powerful 150W Output** – Ensures clear and loud communication  
+- **Built-in Recorder** – Pre-record messages for consistent playback  
+- **Ergonomic Handheld Design** – Comfortable grip for easy portability  
+- **Ideal for Public Use** – Perfect for announcements, rallies &amp; events  
+- **Reliable Sound Amplification** – Projects your voice far &amp; wide  
+Let me know if you'd like any refinements!</t>
+  </si>
+  <si>
+    <t>Here are concise and engaging feature head points for your rechargeable LED flashlight:  
+- **Powerful Beam** – Bright &amp; focused illumination for dark spaces  
+- **USB Rechargeable** – No hassle of replacing batteries, always ready  
+- **Compact &amp; Lightweight** – Easy to carry for outdoor &amp; emergency use  
+- **Durable Design** – Built for longevity &amp; reliable performance  
+- **Versatile Utility** – Ideal for adventures, daily tasks &amp; safety  
+Let me know if you’d like any refinements!</t>
+  </si>
+  <si>
+    <t>Here are impactful feature head points for your scientific calculator:  
+- **Advanced Functions** – Trigonometry, logarithms, exponents &amp; statistics  
+- **User-Friendly Interface** – Simplifies complex calculations effortlessly  
+- **Precision &amp; Efficiency** – Ensures accurate results for math &amp; science  
+- **Durable Design** – Built for long-term professional &amp; academic use  
+- **Versatile Utility** – Ideal for students, professionals &amp; researchers  
+Let me know if you’d like any refinements!</t>
+  </si>
+  <si>
+    <t>Here are concise and engaging feature head points for your 8-in-1 board:  
+- **Multi-Functionality** – Eight integrated tools for enhanced efficiency  
+- **USB Charging Port** – Keep your devices powered with ease  
+- **Compact &amp; Durable** – Designed for home, office &amp; travel convenience  
+- **Streamlined Productivity** – Ideal for multitasking &amp; organized workflow  
+- **Modern &amp; Practical** – The perfect companion for daily use  
+Let me know if you’d like any refinements!</t>
+  </si>
+  <si>
+    <t>Here are sharp and compelling feature head points for your 3-In-1 Torch:  
+- **Powerful Flashlight** – Focused brightness for clear visibility  
+- **Wide-Angle Lamp** – Illuminates larger areas for convenience  
+- **Emergency Strobe Light** – Essential signaling in critical situations  
+- **Rechargeable &amp; Efficient** – Hassle-free power solution for reliability  
+- **Durable &amp; Sleek Design** – Built for longevity with modern aesthetics  
+- **Versatile Utility** – Ideal for outdoor adventures, emergencies &amp; daily use  
+Let me know if you’d like any refinements!</t>
   </si>
 </sst>
 </file>
@@ -838,21 +932,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -881,7 +975,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -910,7 +1004,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -939,7 +1033,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -968,7 +1062,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -997,7 +1091,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1101,7 @@
       <c r="C6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>104</v>
       </c>
       <c r="E6" s="4">
@@ -1026,7 +1120,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1130,7 @@
       <c r="C7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>105</v>
       </c>
       <c r="E7" s="4">
@@ -1055,7 +1149,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1159,7 @@
       <c r="C8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E8" s="4">
@@ -1084,7 +1178,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1109,9 +1203,11 @@
       <c r="H9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1136,9 +1232,11 @@
       <c r="H10" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1163,9 +1261,11 @@
       <c r="H11" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -1190,9 +1290,11 @@
       <c r="H12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -1217,9 +1319,11 @@
       <c r="H13" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -1244,7 +1348,9 @@
       <c r="H14" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1255,23 +1361,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F332D16B-E86D-4EC8-A2D6-D89D89EF2B56}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1282,16 +1391,25 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1301,17 +1419,26 @@
       <c r="C2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="4">
         <v>499</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>249</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -1321,17 +1448,26 @@
       <c r="C3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="4">
         <v>699</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>249</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>59</v>
       </c>
@@ -1341,17 +1477,26 @@
       <c r="C4" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="4">
         <v>299</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>149</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
@@ -1361,17 +1506,26 @@
       <c r="C5" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="4">
         <v>999</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>649</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>61</v>
       </c>
@@ -1381,17 +1535,26 @@
       <c r="C6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="4">
         <v>599</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>199</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>62</v>
       </c>
@@ -1401,17 +1564,26 @@
       <c r="C7" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="4">
         <v>1999</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>999</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>63</v>
       </c>
@@ -1421,17 +1593,26 @@
       <c r="C8" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="4">
         <v>299</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="4">
         <v>199</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>64</v>
       </c>
@@ -1441,17 +1622,26 @@
       <c r="C9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="4">
         <v>999</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>849</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>65</v>
       </c>
@@ -1461,17 +1651,26 @@
       <c r="C10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="4">
         <v>1499</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>999</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>66</v>
       </c>
@@ -1481,14 +1680,23 @@
       <c r="C11" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="4">
         <v>699</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>399</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>85</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>